<commit_message>
add side-bar navigation,semester-wise and section-wise filtering, enhanced UI & readme.md
</commit_message>
<xml_diff>
--- a/backend/output_timetables/sem3_timetable.xlsx
+++ b/backend/output_timetables/sem3_timetable.xlsx
@@ -469,7 +469,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>CS261</t>
+          <t>CS264</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -479,12 +479,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>CS263</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>CS261</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -501,27 +501,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>MA261</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>MA261</t>
-        </is>
-      </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>CS264</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>CS261</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>CS261</t>
+          <t>CS263</t>
         </is>
       </c>
     </row>
@@ -575,17 +575,17 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>MA261</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>CS263</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>CS263</t>
+          <t>CS264</t>
         </is>
       </c>
     </row>
@@ -607,12 +607,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
           <t>CS263</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Free</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -634,7 +634,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>CS261</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -649,7 +649,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>CS264</t>
+          <t>CS261</t>
         </is>
       </c>
     </row>
@@ -707,22 +707,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>CS264</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>CS261</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>CS263</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>CS263</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -749,12 +749,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>CS263</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>CS261</t>
+          <t>CS264</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -803,12 +803,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>CS264</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>MA261</t>
+          <t>CS263</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -823,7 +823,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>CS263</t>
+          <t>CS261</t>
         </is>
       </c>
     </row>
@@ -845,12 +845,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>CS261</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>CS264</t>
+          <t>MA261</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -867,12 +867,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>MA261</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>CS261</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -882,7 +882,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>MA261</t>
+          <t>CS263</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">

</xml_diff>